<commit_message>
repair package issue mesures
</commit_message>
<xml_diff>
--- a/www/mesures/3.0.0/StructureDefinition-mes-diabetis-type.xlsx
+++ b/www/mesures/3.0.0/StructureDefinition-mes-diabetis-type.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-16T15:26:47+01:00</t>
+    <t>2023-03-22T16:32:25+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1113,7 +1113,7 @@
         <v>74</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>92</v>
@@ -1319,7 +1319,7 @@
         <v>79</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>105</v>
@@ -1424,7 +1424,7 @@
         <v>79</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AJ7" t="s" s="2">
         <v>105</v>

</xml_diff>